<commit_message>
đã fix lỗi, check cho cả domestic và other
</commit_message>
<xml_diff>
--- a/Data/applications.xlsx
+++ b/Data/applications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\UiPath\RPA_CreditCardApproval\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8543DDA2-D589-419D-8BEB-0E4172E192CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADE4CD5-9D83-4E00-8709-842B953E2223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E97AD6F-C8ED-41E8-A99D-529865D1ED40}"/>
   </bookViews>
@@ -1069,7 +1069,7 @@
   <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,7 +1078,12 @@
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="11" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" customWidth="1"/>
+    <col min="9" max="9" width="50" customWidth="1"/>
+    <col min="10" max="11" width="14.6640625" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" style="19" customWidth="1"/>
     <col min="13" max="14" width="20.44140625" customWidth="1"/>
     <col min="15" max="16" width="14.6640625" customWidth="1"/>

</xml_diff>